<commit_message>
minor changes to jmeter scripts and feature
</commit_message>
<xml_diff>
--- a/src/test/resources/config/data/NB/1/manuallyCalcDif.xlsx
+++ b/src/test/resources/config/data/NB/1/manuallyCalcDif.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="40">
   <si>
     <t>Subscriber</t>
   </si>
@@ -50,103 +50,88 @@
     <t>AutInvSP3</t>
   </si>
   <si>
+    <t>AutInvSP3_AutInvSP4_app4</t>
+  </si>
+  <si>
+    <t>smsmessaging</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>Send SMS</t>
+  </si>
+  <si>
+    <t>SM1</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Rs 0.0</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Retrive SMS</t>
+  </si>
+  <si>
+    <t>SM2</t>
+  </si>
+  <si>
+    <t>Query SMS Delivery</t>
+  </si>
+  <si>
+    <t>Delivery Subscription</t>
+  </si>
+  <si>
+    <t>Stop Delivery Subscription</t>
+  </si>
+  <si>
+    <t>Retrive SMS Subscription</t>
+  </si>
+  <si>
+    <t>Stop Retrive SMS Subscription</t>
+  </si>
+  <si>
+    <t>SMS Inbound Notification</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>AutInvSP3_AutInvSP3_app3</t>
+  </si>
+  <si>
+    <t>AutInvSP3_AutInvSP3_app2</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>Refund</t>
+  </si>
+  <si>
+    <t>RF2</t>
+  </si>
+  <si>
+    <t>ussd</t>
+  </si>
+  <si>
+    <t>Send USSD</t>
+  </si>
+  <si>
+    <t>u1</t>
+  </si>
+  <si>
     <t>AutInvSP3_AutInvSP3_app1</t>
-  </si>
-  <si>
-    <t>smsmessaging</t>
-  </si>
-  <si>
-    <t>v1</t>
-  </si>
-  <si>
-    <t>Send SMS</t>
-  </si>
-  <si>
-    <t>SM1</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>Rs 0.0</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Retrive SMS</t>
-  </si>
-  <si>
-    <t>SM2</t>
-  </si>
-  <si>
-    <t>Query SMS Delivery</t>
-  </si>
-  <si>
-    <t>Delivery Subscription</t>
-  </si>
-  <si>
-    <t>Stop Delivery Subscription</t>
-  </si>
-  <si>
-    <t>Retrive SMS Subscription</t>
-  </si>
-  <si>
-    <t>Stop Retrive SMS Subscription</t>
-  </si>
-  <si>
-    <t>SMS Inbound Notification</t>
-  </si>
-  <si>
-    <t>payment</t>
-  </si>
-  <si>
-    <t>Charge</t>
-  </si>
-  <si>
-    <t>p1</t>
-  </si>
-  <si>
-    <t>Refund</t>
-  </si>
-  <si>
-    <t>RF2</t>
-  </si>
-  <si>
-    <t>ussd</t>
-  </si>
-  <si>
-    <t>Send USSD</t>
-  </si>
-  <si>
-    <t>u1</t>
-  </si>
-  <si>
-    <t>Total Amount</t>
-  </si>
-  <si>
-    <t>Rs 70.0</t>
-  </si>
-  <si>
-    <t>Rs 7.5</t>
-  </si>
-  <si>
-    <t>AutInvSP3_AutInvSP3_app3</t>
-  </si>
-  <si>
-    <t>Rs 8.0</t>
-  </si>
-  <si>
-    <t>Rs 1.5</t>
-  </si>
-  <si>
-    <t>AutInvSP3_AutInvSP4_app4</t>
-  </si>
-  <si>
-    <t>Rs -72.0</t>
-  </si>
-  <si>
-    <t>Rs -6.0</t>
   </si>
 </sst>
 </file>
@@ -520,20 +505,20 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
       <c r="H10" t="s">
         <v>18</v>
       </c>
@@ -544,7 +529,7 @@
         <v>18</v>
       </c>
       <c r="K10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -552,19 +537,19 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
         <v>17</v>
@@ -590,16 +575,16 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
@@ -631,25 +616,25 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="I13" t="s">
         <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -657,19 +642,19 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
         <v>17</v>
@@ -701,7 +686,7 @@
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
@@ -736,7 +721,7 @@
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
@@ -771,7 +756,7 @@
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
@@ -806,7 +791,7 @@
         <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
         <v>21</v>
@@ -841,13 +826,13 @@
         <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
@@ -859,7 +844,7 @@
         <v>18</v>
       </c>
       <c r="K19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
@@ -876,13 +861,13 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H20" t="s">
         <v>18</v>
@@ -894,7 +879,7 @@
         <v>18</v>
       </c>
       <c r="K20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
@@ -902,19 +887,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="G21" t="s">
         <v>17</v>
@@ -946,25 +931,25 @@
         <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G22" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H22" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I22" t="s">
         <v>18</v>
       </c>
       <c r="J22" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="K22" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
@@ -972,7 +957,7 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -1255,16 +1240,16 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F31" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G31" t="s">
         <v>17</v>
@@ -1296,13 +1281,13 @@
         <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H32" t="s">
         <v>18</v>
@@ -1314,7 +1299,7 @@
         <v>18</v>
       </c>
       <c r="K32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33">
@@ -1322,19 +1307,19 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G33" t="s">
         <v>17</v>
@@ -1366,25 +1351,375 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F34" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" t="s">
+        <v>18</v>
+      </c>
+      <c r="K34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" t="s">
+        <v>18</v>
+      </c>
+      <c r="K40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" t="s">
+        <v>18</v>
+      </c>
+      <c r="K42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
         <v>36</v>
       </c>
-      <c r="H34" t="s">
-        <v>43</v>
-      </c>
-      <c r="I34" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" t="s">
-        <v>44</v>
-      </c>
-      <c r="K34" t="s">
-        <v>43</v>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" t="s">
+        <v>18</v>
+      </c>
+      <c r="K44" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>